<commit_message>
Burdel na kółkach, ale chociaż import z weksela działa
</commit_message>
<xml_diff>
--- a/Code/data.xlsx
+++ b/Code/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="README"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3534" uniqueCount="3044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3549" uniqueCount="3044">
   <si>
     <t>README</t>
   </si>
@@ -9252,7 +9252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -9261,13 +9261,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -9581,25 +9587,25 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>3036</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>3037</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="1" t="s">
         <v>3038</v>
       </c>
@@ -9608,47 +9614,47 @@
       <c r="A3" s="1" t="s">
         <v>3039</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>3040</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>3041</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>3042</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>3043</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9673,14 +9679,16 @@
     <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="4"/>
+      <c r="A1" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>1264</v>
       </c>
@@ -9822,14 +9830,14 @@
       <c r="E6" s="1" t="s">
         <v>1327</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="1" t="s">
         <v>1328</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>1329</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
@@ -9897,14 +9905,14 @@
       <c r="E9" s="1" t="s">
         <v>1345</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="1" t="s">
         <v>1346</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>1347</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9934,7 +9942,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>1264</v>
       </c>
@@ -10094,7 +10104,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>1264</v>
       </c>
@@ -10203,7 +10215,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>163</v>
       </c>
@@ -11610,7 +11624,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>163</v>
       </c>
@@ -12657,7 +12673,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>164</v>
       </c>
@@ -13398,7 +13416,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>177</v>
       </c>
@@ -13887,7 +13907,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>182</v>
       </c>
@@ -14170,15 +14192,17 @@
   <cols>
     <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="4"/>
+      <c r="A1" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>191</v>
       </c>
@@ -14222,15 +14246,15 @@
       <c r="B3" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
@@ -14256,15 +14280,15 @@
       <c r="B5" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
@@ -14290,15 +14314,15 @@
       <c r="B7" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14909,7 +14933,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="58.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="58.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="45.75">
@@ -15317,7 +15341,7 @@
   </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15619,7 +15643,7 @@
   </sheetPr>
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>
@@ -17237,7 +17261,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>81</v>
       </c>
@@ -18559,7 +18585,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>86</v>
       </c>
@@ -19643,7 +19671,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
@@ -20513,7 +20543,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
@@ -21193,7 +21225,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="4"/>
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
@@ -21700,14 +21734,16 @@
     <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="4"/>
+      <c r="A1" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>110</v>
       </c>
@@ -21947,14 +21983,14 @@
       <c r="G8" s="1" t="s">
         <v>1402</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="1" t="s">
         <v>1403</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>1404</v>
       </c>
-      <c r="K8" s="4"/>
+      <c r="K8" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
@@ -22040,14 +22076,14 @@
       <c r="G11" s="1" t="s">
         <v>1426</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="1" t="s">
         <v>1427</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>1428</v>
       </c>
-      <c r="K11" s="4"/>
+      <c r="K11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>